<commit_message>
Diode testing working. External button interrupt for diode switch done
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DesCon\DMM-STM32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrik\Development\DMM-STM32\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="131">
   <si>
     <t>J7</t>
   </si>
@@ -56,33 +56,6 @@
     <t xml:space="preserve">Range 0 (Gain 1) </t>
   </si>
   <si>
-    <t>GPIO1</t>
-  </si>
-  <si>
-    <t>GPIO2</t>
-  </si>
-  <si>
-    <t>GPIO3</t>
-  </si>
-  <si>
-    <t>GPIO4</t>
-  </si>
-  <si>
-    <t>1&lt;&lt;3</t>
-  </si>
-  <si>
-    <t>GPIO5</t>
-  </si>
-  <si>
-    <t>2 &lt;&lt;3</t>
-  </si>
-  <si>
-    <t>3 &lt;&lt;3</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
     <t>Range</t>
   </si>
   <si>
@@ -329,21 +302,6 @@
     <t>~(1 &lt;&lt; 8)</t>
   </si>
   <si>
-    <t>GPIO6</t>
-  </si>
-  <si>
-    <t>GPIO7</t>
-  </si>
-  <si>
-    <t>GPIO8</t>
-  </si>
-  <si>
-    <t>GPIO9</t>
-  </si>
-  <si>
-    <t>1&lt;&lt;</t>
-  </si>
-  <si>
     <t>(1&lt;&lt;8)</t>
   </si>
   <si>
@@ -407,7 +365,58 @@
     <t>~(1&lt;&lt;7),(2&lt;&lt;4)</t>
   </si>
   <si>
-    <t>;</t>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>Diode DTM Mode</t>
+  </si>
+  <si>
+    <t>Diode ZDT Mode</t>
+  </si>
+  <si>
+    <t>Diode test A1 Input</t>
+  </si>
+  <si>
+    <t>Diode Test A2 Input</t>
+  </si>
+  <si>
+    <t>Diode Test A3 Input</t>
+  </si>
+  <si>
+    <t>Diode Test A0 Input</t>
+  </si>
+  <si>
+    <t>DIODE_A3_IN</t>
+  </si>
+  <si>
+    <t>DIODE_A2_IN</t>
+  </si>
+  <si>
+    <t>DIODE_A1_IN</t>
+  </si>
+  <si>
+    <t>DIODE_A0_IN</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>~(1&lt;&lt;1)</t>
+  </si>
+  <si>
+    <t>(1&lt;&lt;1)</t>
   </si>
 </sst>
 </file>
@@ -444,7 +453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +520,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF000F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -873,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1162,11 +1177,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1207,14 +1225,39 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,8 +1267,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF000F0"/>
       <color rgb="FFFFB9FF"/>
-      <color rgb="FFF000F0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1502,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R63"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,31 +1581,31 @@
         <v>6</v>
       </c>
       <c r="F1" s="101" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="49" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="K1" s="51" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
-        <v>19</v>
+      <c r="A2" s="112" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1570,14 +1613,14 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="112" t="s">
-        <v>99</v>
+      <c r="F2" s="131" t="s">
+        <v>90</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J2" s="36">
         <v>1</v>
@@ -1585,10 +1628,10 @@
       <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="128"/>
+      <c r="A3" s="113"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
@@ -1596,7 +1639,7 @@
       <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="113"/>
+      <c r="F3" s="132"/>
       <c r="I3" s="38"/>
       <c r="J3" s="34">
         <v>2</v>
@@ -1604,12 +1647,12 @@
       <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -1617,22 +1660,22 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="112" t="s">
-        <v>123</v>
+      <c r="F4" s="131" t="s">
+        <v>109</v>
       </c>
       <c r="I4" s="38"/>
       <c r="J4" s="55">
         <v>3</v>
       </c>
       <c r="K4" s="58" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="128"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
@@ -1640,22 +1683,22 @@
       <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="113"/>
+      <c r="F5" s="132"/>
       <c r="I5" s="38"/>
       <c r="J5" s="55">
         <v>4</v>
       </c>
       <c r="K5" s="58" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="128"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -1663,22 +1706,22 @@
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="112" t="s">
-        <v>124</v>
+      <c r="F6" s="131" t="s">
+        <v>110</v>
       </c>
       <c r="I6" s="38"/>
       <c r="J6" s="55">
         <v>5</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="128"/>
+      <c r="A7" s="113"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
@@ -1686,22 +1729,22 @@
       <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="132"/>
       <c r="I7" s="38"/>
       <c r="J7" s="54">
         <v>6</v>
       </c>
       <c r="K7" s="72" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -1709,22 +1752,22 @@
       <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="112" t="s">
-        <v>125</v>
+      <c r="F8" s="131" t="s">
+        <v>111</v>
       </c>
       <c r="I8" s="38"/>
       <c r="J8" s="92">
         <v>7</v>
       </c>
       <c r="K8" s="93" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="128"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
@@ -1732,7 +1775,7 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="113"/>
+      <c r="F9" s="132"/>
       <c r="I9" s="40"/>
       <c r="J9" s="41">
         <v>8</v>
@@ -1740,27 +1783,27 @@
       <c r="K9" s="42"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="128"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
       </c>
       <c r="F10" s="105" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="J10" s="36">
         <v>1</v>
@@ -1768,21 +1811,21 @@
       <c r="K10" s="37"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="129"/>
+      <c r="A11" s="114"/>
       <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E11" s="14">
         <v>1</v>
       </c>
       <c r="F11" s="105" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="34">
@@ -1792,138 +1835,138 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="88" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B12" s="89"/>
       <c r="C12" s="90" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D12" s="90" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F12" s="105"/>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="95">
         <v>3</v>
       </c>
       <c r="K12" s="96" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="124" t="s">
-        <v>32</v>
+      <c r="A13" s="125" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="109" t="s">
-        <v>107</v>
+      <c r="F13" s="128" t="s">
+        <v>93</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="70">
         <v>4</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="125"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E14" s="20">
         <v>0</v>
       </c>
-      <c r="F14" s="111"/>
+      <c r="F14" s="130"/>
       <c r="I14" s="43"/>
       <c r="J14" s="70">
         <v>5</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="15" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="109" t="s">
-        <v>108</v>
+      <c r="F15" s="128" t="s">
+        <v>94</v>
       </c>
       <c r="I15" s="43"/>
       <c r="J15" s="70">
         <v>6</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="125"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E16" s="20">
         <v>1</v>
       </c>
-      <c r="F16" s="111"/>
+      <c r="F16" s="130"/>
       <c r="I16" s="43"/>
       <c r="J16" s="34">
         <v>7</v>
       </c>
       <c r="K16" s="44"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="125"/>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="126"/>
       <c r="B17" s="15" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E17" s="17">
         <v>1</v>
       </c>
-      <c r="F17" s="109" t="s">
-        <v>109</v>
+      <c r="F17" s="128" t="s">
+        <v>95</v>
       </c>
       <c r="I17" s="45"/>
       <c r="J17" s="41">
@@ -1932,19 +1975,19 @@
       <c r="K17" s="46"/>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="125"/>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="126"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E18" s="20">
         <v>0</v>
       </c>
-      <c r="F18" s="111"/>
+      <c r="F18" s="130"/>
       <c r="I18" s="47" t="s">
         <v>0</v>
       </c>
@@ -1954,22 +1997,22 @@
       <c r="K18" s="48"/>
       <c r="M18" s="33"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="126"/>
       <c r="B19" s="21" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E19" s="23">
         <v>1</v>
       </c>
-      <c r="F19" s="109" t="s">
-        <v>110</v>
+      <c r="F19" s="128" t="s">
+        <v>96</v>
       </c>
       <c r="I19" s="43"/>
       <c r="J19" s="52">
@@ -1980,19 +2023,19 @@
       </c>
       <c r="M19" s="33"/>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="126"/>
+    <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="127"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E20" s="20">
         <v>1</v>
       </c>
-      <c r="F20" s="111"/>
+      <c r="F20" s="130"/>
       <c r="I20" s="43"/>
       <c r="J20" s="52">
         <v>3</v>
@@ -2002,98 +2045,96 @@
       </c>
       <c r="M20" s="33"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="122" t="s">
-        <v>42</v>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="123" t="s">
+        <v>33</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E21" s="26">
         <v>0</v>
       </c>
-      <c r="F21" s="109" t="s">
-        <v>112</v>
+      <c r="F21" s="128" t="s">
+        <v>98</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="56">
         <v>4</v>
       </c>
       <c r="K21" s="57" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="M21" s="33"/>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="123"/>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="124"/>
       <c r="B22" s="24"/>
       <c r="C22" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E22" s="26">
         <v>0</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="129"/>
       <c r="I22" s="43"/>
       <c r="J22" s="56">
         <v>5</v>
       </c>
       <c r="K22" s="57" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M22" s="33"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="124"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="E23" s="29">
         <v>0</v>
       </c>
-      <c r="F23" s="111"/>
+      <c r="F23" s="130"/>
       <c r="I23" s="43"/>
       <c r="J23" s="73">
         <v>6</v>
       </c>
       <c r="K23" s="74" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="M23" s="33"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="124"/>
       <c r="B24" s="30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E24" s="32">
         <v>0</v>
       </c>
-      <c r="F24" s="109" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>127</v>
-      </c>
+      <c r="F24" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="139"/>
       <c r="I24" s="43"/>
       <c r="J24" s="34">
         <v>7</v>
@@ -2101,19 +2142,19 @@
       <c r="K24" s="44"/>
       <c r="M24" s="33"/>
     </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="123"/>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="124"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E25" s="26">
         <v>0</v>
       </c>
-      <c r="F25" s="110"/>
+      <c r="F25" s="129"/>
       <c r="I25" s="45"/>
       <c r="J25" s="41">
         <v>8</v>
@@ -2121,708 +2162,723 @@
       <c r="K25" s="46"/>
       <c r="M25" s="33"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="123"/>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="124"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>55</v>
       </c>
       <c r="E26" s="29">
         <v>1</v>
       </c>
-      <c r="F26" s="111"/>
+      <c r="F26" s="130"/>
       <c r="M26" s="33"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="124"/>
       <c r="B27" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>44</v>
-      </c>
       <c r="D27" s="25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E27" s="32">
         <v>0</v>
       </c>
-      <c r="F27" s="109" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27" t="s">
-        <v>104</v>
-      </c>
-      <c r="K27" t="s">
-        <v>103</v>
-      </c>
-      <c r="L27" t="s">
-        <v>102</v>
-      </c>
-      <c r="M27" t="s">
-        <v>101</v>
-      </c>
-      <c r="N27" t="s">
-        <v>15</v>
-      </c>
-      <c r="O27" t="s">
-        <v>13</v>
-      </c>
-      <c r="P27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>11</v>
-      </c>
-      <c r="R27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="123"/>
+      <c r="F27" s="128" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="124"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E28" s="26">
         <v>1</v>
       </c>
-      <c r="F28" s="110"/>
-      <c r="I28" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="2">
-        <v>0</v>
-      </c>
-      <c r="O28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="123"/>
+      <c r="F28" s="129"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="124"/>
       <c r="B29" s="27"/>
       <c r="C29" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="E29" s="29">
         <v>0</v>
       </c>
-      <c r="F29" s="111"/>
-      <c r="I29" t="s">
-        <v>14</v>
-      </c>
-      <c r="N29" s="2">
-        <v>0</v>
-      </c>
-      <c r="O29" s="2">
-        <v>1</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="123"/>
+      <c r="F29" s="130"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="124"/>
       <c r="B30" s="30" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E30" s="32">
         <v>0</v>
       </c>
-      <c r="F30" s="109" t="s">
-        <v>114</v>
-      </c>
-      <c r="I30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="2">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
+      <c r="F30" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="124"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E31" s="26">
         <v>1</v>
       </c>
-      <c r="F31" s="110"/>
-      <c r="I31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
+      <c r="F31" s="129"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="124"/>
       <c r="B32" s="27"/>
       <c r="C32" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>55</v>
       </c>
       <c r="E32" s="29">
         <v>1</v>
       </c>
-      <c r="F32" s="111"/>
-      <c r="I32" t="s">
-        <v>105</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
+      <c r="F32" s="130"/>
       <c r="M32" s="33"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="123"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="30" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E33" s="32">
         <v>1</v>
       </c>
-      <c r="F33" s="109" t="s">
-        <v>111</v>
+      <c r="F33" s="128" t="s">
+        <v>97</v>
       </c>
       <c r="M33" s="33"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="123"/>
+      <c r="A34" s="124"/>
       <c r="B34" s="24"/>
       <c r="C34" s="25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E34" s="26">
         <v>0</v>
       </c>
-      <c r="F34" s="110"/>
+      <c r="F34" s="129"/>
       <c r="M34" s="33"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="123"/>
+      <c r="A35" s="124"/>
       <c r="B35" s="24"/>
       <c r="C35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="25" t="s">
-        <v>55</v>
-      </c>
       <c r="E35" s="26">
         <v>0</v>
       </c>
-      <c r="F35" s="111"/>
+      <c r="F35" s="130"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="97" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B36" s="98" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C36" s="99" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D36" s="99" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E36" s="100" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F36" s="106"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="117" t="s">
-        <v>48</v>
+      <c r="A37" s="118" t="s">
+        <v>39</v>
       </c>
       <c r="B37" s="64" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C37" s="60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D37" s="60" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E37" s="67">
         <v>0</v>
       </c>
-      <c r="F37" s="109" t="s">
-        <v>115</v>
+      <c r="F37" s="128" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="118"/>
+      <c r="A38" s="119"/>
       <c r="B38" s="65"/>
       <c r="C38" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D38" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E38" s="68">
         <v>0</v>
       </c>
-      <c r="F38" s="110"/>
+      <c r="F38" s="129"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="118"/>
+      <c r="A39" s="119"/>
       <c r="B39" s="66"/>
       <c r="C39" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D39" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E39" s="69">
         <v>0</v>
       </c>
-      <c r="F39" s="111"/>
+      <c r="F39" s="130"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="118"/>
+      <c r="A40" s="119"/>
       <c r="B40" s="64" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C40" s="60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D40" s="60" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E40" s="67">
         <v>0</v>
       </c>
-      <c r="F40" s="109" t="s">
-        <v>116</v>
+      <c r="F40" s="128" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="118"/>
+      <c r="A41" s="119"/>
       <c r="B41" s="65"/>
       <c r="C41" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D41" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E41" s="68">
         <v>0</v>
       </c>
-      <c r="F41" s="110"/>
+      <c r="F41" s="129"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="118"/>
+      <c r="A42" s="119"/>
       <c r="B42" s="66"/>
       <c r="C42" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E42" s="69">
         <v>1</v>
       </c>
-      <c r="F42" s="111"/>
+      <c r="F42" s="130"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="118"/>
+      <c r="A43" s="119"/>
       <c r="B43" s="64" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C43" s="60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D43" s="60" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E43" s="67">
         <v>0</v>
       </c>
-      <c r="F43" s="109" t="s">
-        <v>117</v>
+      <c r="F43" s="128" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="118"/>
+      <c r="A44" s="119"/>
       <c r="B44" s="65"/>
       <c r="C44" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D44" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E44" s="68">
         <v>1</v>
       </c>
-      <c r="F44" s="110"/>
+      <c r="F44" s="129"/>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="118"/>
+      <c r="A45" s="119"/>
       <c r="B45" s="66"/>
       <c r="C45" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D45" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E45" s="69">
         <v>0</v>
       </c>
-      <c r="F45" s="111"/>
+      <c r="F45" s="130"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="118"/>
+      <c r="A46" s="119"/>
       <c r="B46" s="64" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D46" s="60" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E46" s="67">
         <v>0</v>
       </c>
-      <c r="F46" s="109" t="s">
-        <v>118</v>
+      <c r="F46" s="128" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="118"/>
+      <c r="A47" s="119"/>
       <c r="B47" s="65"/>
       <c r="C47" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D47" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E47" s="68">
         <v>1</v>
       </c>
-      <c r="F47" s="110"/>
+      <c r="F47" s="129"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="118"/>
+      <c r="A48" s="119"/>
       <c r="B48" s="66"/>
       <c r="C48" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D48" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E48" s="69">
         <v>1</v>
       </c>
-      <c r="F48" s="111"/>
+      <c r="F48" s="130"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="118"/>
+      <c r="A49" s="119"/>
       <c r="B49" s="64" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C49" s="60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D49" s="60" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E49" s="67">
         <v>1</v>
       </c>
-      <c r="F49" s="109" t="s">
-        <v>119</v>
+      <c r="F49" s="128" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="118"/>
+      <c r="A50" s="119"/>
       <c r="B50" s="65"/>
       <c r="C50" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D50" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E50" s="68">
         <v>0</v>
       </c>
-      <c r="F50" s="110"/>
+      <c r="F50" s="129"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="118"/>
+      <c r="A51" s="119"/>
       <c r="B51" s="66"/>
       <c r="C51" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D51" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E51" s="69">
         <v>0</v>
       </c>
-      <c r="F51" s="111"/>
+      <c r="F51" s="130"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="118"/>
+      <c r="A52" s="119"/>
       <c r="B52" s="61" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C52" s="59" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D52" s="59" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E52" s="68">
         <v>1</v>
       </c>
-      <c r="F52" s="109" t="s">
-        <v>120</v>
+      <c r="F52" s="128" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="118"/>
+      <c r="A53" s="119"/>
       <c r="B53" s="61"/>
       <c r="C53" s="59" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D53" s="59" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E53" s="68">
         <v>0</v>
       </c>
-      <c r="F53" s="110"/>
+      <c r="F53" s="129"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="119"/>
+      <c r="A54" s="120"/>
       <c r="B54" s="62"/>
       <c r="C54" s="63" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D54" s="63" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E54" s="69">
         <v>1</v>
       </c>
-      <c r="F54" s="111"/>
+      <c r="F54" s="130"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="120" t="s">
-        <v>70</v>
+      <c r="A55" s="121" t="s">
+        <v>61</v>
       </c>
       <c r="B55" s="102" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C55" s="103" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D55" s="103" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E55" s="104">
         <v>0</v>
       </c>
       <c r="F55" s="105" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="121"/>
+      <c r="A56" s="122"/>
       <c r="B56" s="75" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C56" s="76" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D56" s="76" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E56" s="77">
         <v>1</v>
       </c>
       <c r="F56" s="107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="133" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="134" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="135" t="s">
+        <v>128</v>
+      </c>
+      <c r="E57" s="136">
+        <v>0</v>
+      </c>
+      <c r="F57" s="109" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="137"/>
+      <c r="B58" s="134" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="135" t="s">
+        <v>128</v>
+      </c>
+      <c r="E58" s="136">
+        <v>1</v>
+      </c>
+      <c r="F58" s="110" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="137"/>
+      <c r="B59" s="134" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="135" t="s">
+        <v>127</v>
+      </c>
+      <c r="E59" s="136" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="110"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="137"/>
+      <c r="B60" s="134" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="135" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="136" t="s">
+        <v>121</v>
+      </c>
+      <c r="F60" s="110"/>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="137"/>
+      <c r="B61" s="134" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="135" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" s="136" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="114" t="s">
+      <c r="F61" s="110"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="138"/>
+      <c r="B62" s="134" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="135" t="s">
+        <v>124</v>
+      </c>
+      <c r="E62" s="136" t="s">
+        <v>123</v>
+      </c>
+      <c r="F62" s="111"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="81" t="s">
+      <c r="E63" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" s="105"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="116"/>
+      <c r="B64" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="107"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="116"/>
+      <c r="B65" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="82" t="s">
+      <c r="E65" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" s="107"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="116"/>
+      <c r="B66" s="81" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="87"/>
+      <c r="F66" s="106"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="116"/>
+      <c r="B67" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="D57" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="83" t="s">
+      <c r="C67" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" s="86"/>
+      <c r="F67" s="108"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="116"/>
+      <c r="B68" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68" s="87"/>
+      <c r="F68" s="107"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="117"/>
+      <c r="B69" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="F57" s="105"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="115"/>
-      <c r="B58" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="E58" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="F58" s="107"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
-      <c r="B59" s="84" t="s">
+      <c r="C69" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="C59" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="85" t="s">
+      <c r="D69" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="E59" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="F59" s="107"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="115"/>
-      <c r="B60" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="82" t="s">
-        <v>91</v>
-      </c>
-      <c r="E60" s="87"/>
-      <c r="F60" s="106"/>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="115"/>
-      <c r="B61" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="C61" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="E61" s="86"/>
-      <c r="F61" s="108"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="115"/>
-      <c r="B62" s="81" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="82" t="s">
-        <v>90</v>
-      </c>
-      <c r="D62" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="87"/>
-      <c r="F62" s="107"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="116"/>
-      <c r="B63" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="86"/>
-      <c r="F63" s="108"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="108"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="A37:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A21:A35"/>
-    <mergeCell ref="A13:A20"/>
+  <mergeCells count="26">
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F49:F51"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
@@ -2835,13 +2891,13 @@
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="A37:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A21:A35"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A57:A62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
WE'RE FUCKING DONE MAN
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrik\Development\DMM-STM32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DesCon\DMM-STM32\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="132">
   <si>
     <t>J7</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>(1&lt;&lt;1)</t>
+  </si>
+  <si>
+    <t>(3&lt;&lt;5),~(1&lt;&lt;5)</t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1051,7 +1054,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1149,13 +1151,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1187,6 +1182,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1202,63 +1257,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1545,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,19 +1570,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="F1" s="100" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1598,7 +1600,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="113" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1613,7 +1615,7 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="135" t="s">
         <v>90</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -1628,7 +1630,7 @@
       <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="122"/>
+      <c r="A3" s="114"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>31</v>
@@ -1639,7 +1641,7 @@
       <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="120"/>
+      <c r="F3" s="136"/>
       <c r="I3" s="38"/>
       <c r="J3" s="34">
         <v>2</v>
@@ -1647,7 +1649,7 @@
       <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
+      <c r="A4" s="114"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1660,7 +1662,7 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="119" t="s">
+      <c r="F4" s="135" t="s">
         <v>109</v>
       </c>
       <c r="I4" s="38"/>
@@ -1672,7 +1674,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122"/>
+      <c r="A5" s="114"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>31</v>
@@ -1683,7 +1685,7 @@
       <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="120"/>
+      <c r="F5" s="136"/>
       <c r="I5" s="38"/>
       <c r="J5" s="55">
         <v>4</v>
@@ -1693,7 +1695,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
+      <c r="A6" s="114"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1706,7 +1708,7 @@
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="119" t="s">
+      <c r="F6" s="135" t="s">
         <v>110</v>
       </c>
       <c r="I6" s="38"/>
@@ -1718,7 +1720,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="122"/>
+      <c r="A7" s="114"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
         <v>31</v>
@@ -1729,17 +1731,17 @@
       <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="120"/>
+      <c r="F7" s="136"/>
       <c r="I7" s="38"/>
       <c r="J7" s="54">
         <v>6</v>
       </c>
-      <c r="K7" s="72" t="s">
+      <c r="K7" s="71" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
+      <c r="A8" s="114"/>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1752,19 +1754,19 @@
       <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="119" t="s">
+      <c r="F8" s="135" t="s">
         <v>111</v>
       </c>
       <c r="I8" s="38"/>
-      <c r="J8" s="92">
+      <c r="J8" s="91">
         <v>7</v>
       </c>
-      <c r="K8" s="93" t="s">
+      <c r="K8" s="92" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="122"/>
+      <c r="A9" s="114"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
         <v>31</v>
@@ -1775,7 +1777,7 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="120"/>
+      <c r="F9" s="136"/>
       <c r="I9" s="40"/>
       <c r="J9" s="41">
         <v>8</v>
@@ -1783,7 +1785,7 @@
       <c r="K9" s="42"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="122"/>
+      <c r="A10" s="114"/>
       <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1798,7 @@
       <c r="E10" s="11">
         <v>0</v>
       </c>
-      <c r="F10" s="105" t="s">
+      <c r="F10" s="101" t="s">
         <v>91</v>
       </c>
       <c r="G10" s="13" t="s">
@@ -1811,7 +1813,7 @@
       <c r="K10" s="37"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="123"/>
+      <c r="A11" s="115"/>
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
@@ -1824,7 +1826,7 @@
       <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="101" t="s">
         <v>92</v>
       </c>
       <c r="I11" s="43"/>
@@ -1834,33 +1836,33 @@
       <c r="K11" s="44"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="90" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="91" t="s">
+      <c r="E12" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="105"/>
+      <c r="F12" s="101"/>
       <c r="G12" t="s">
         <v>65</v>
       </c>
       <c r="I12" s="43"/>
-      <c r="J12" s="95">
+      <c r="J12" s="94">
         <v>3</v>
       </c>
-      <c r="K12" s="96" t="s">
+      <c r="K12" s="95" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="126" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -1875,19 +1877,19 @@
       <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="116" t="s">
+      <c r="F13" s="132" t="s">
         <v>93</v>
       </c>
       <c r="I13" s="43"/>
-      <c r="J13" s="70">
+      <c r="J13" s="69">
         <v>4</v>
       </c>
-      <c r="K13" s="71" t="s">
+      <c r="K13" s="70" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
         <v>14</v>
@@ -1898,17 +1900,17 @@
       <c r="E14" s="20">
         <v>0</v>
       </c>
-      <c r="F14" s="118"/>
+      <c r="F14" s="134"/>
       <c r="I14" s="43"/>
-      <c r="J14" s="70">
+      <c r="J14" s="69">
         <v>5</v>
       </c>
-      <c r="K14" s="71" t="s">
+      <c r="K14" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
@@ -1921,19 +1923,19 @@
       <c r="E15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="116" t="s">
+      <c r="F15" s="132" t="s">
         <v>94</v>
       </c>
       <c r="I15" s="43"/>
-      <c r="J15" s="70">
+      <c r="J15" s="69">
         <v>6</v>
       </c>
-      <c r="K15" s="71" t="s">
+      <c r="K15" s="70" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="135"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
         <v>14</v>
@@ -1944,7 +1946,7 @@
       <c r="E16" s="20">
         <v>1</v>
       </c>
-      <c r="F16" s="118"/>
+      <c r="F16" s="134"/>
       <c r="I16" s="43"/>
       <c r="J16" s="34">
         <v>7</v>
@@ -1952,7 +1954,7 @@
       <c r="K16" s="44"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="135"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="15" t="s">
         <v>29</v>
       </c>
@@ -1965,7 +1967,7 @@
       <c r="E17" s="17">
         <v>1</v>
       </c>
-      <c r="F17" s="116" t="s">
+      <c r="F17" s="132" t="s">
         <v>95</v>
       </c>
       <c r="I17" s="45"/>
@@ -1976,7 +1978,7 @@
       <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="135"/>
+      <c r="A18" s="127"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
         <v>14</v>
@@ -1987,7 +1989,7 @@
       <c r="E18" s="20">
         <v>0</v>
       </c>
-      <c r="F18" s="118"/>
+      <c r="F18" s="134"/>
       <c r="I18" s="47" t="s">
         <v>0</v>
       </c>
@@ -1998,7 +2000,7 @@
       <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="135"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="21" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2013,7 @@
       <c r="E19" s="23">
         <v>1</v>
       </c>
-      <c r="F19" s="116" t="s">
+      <c r="F19" s="132" t="s">
         <v>96</v>
       </c>
       <c r="I19" s="43"/>
@@ -2024,7 +2026,7 @@
       <c r="M19" s="33"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136"/>
+      <c r="A20" s="128"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
         <v>14</v>
@@ -2035,7 +2037,7 @@
       <c r="E20" s="20">
         <v>1</v>
       </c>
-      <c r="F20" s="118"/>
+      <c r="F20" s="134"/>
       <c r="I20" s="43"/>
       <c r="J20" s="52">
         <v>3</v>
@@ -2046,7 +2048,7 @@
       <c r="M20" s="33"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="132" t="s">
+      <c r="A21" s="124" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -2061,7 +2063,7 @@
       <c r="E21" s="26">
         <v>0</v>
       </c>
-      <c r="F21" s="116" t="s">
+      <c r="F21" s="132" t="s">
         <v>98</v>
       </c>
       <c r="I21" s="43"/>
@@ -2074,7 +2076,7 @@
       <c r="M21" s="33"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="24"/>
       <c r="C22" s="25" t="s">
         <v>36</v>
@@ -2085,7 +2087,7 @@
       <c r="E22" s="26">
         <v>0</v>
       </c>
-      <c r="F22" s="117"/>
+      <c r="F22" s="133"/>
       <c r="I22" s="43"/>
       <c r="J22" s="56">
         <v>5</v>
@@ -2096,7 +2098,7 @@
       <c r="M22" s="33"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="133"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28" t="s">
         <v>37</v>
@@ -2107,18 +2109,18 @@
       <c r="E23" s="29">
         <v>0</v>
       </c>
-      <c r="F23" s="118"/>
+      <c r="F23" s="134"/>
       <c r="I23" s="43"/>
-      <c r="J23" s="73">
+      <c r="J23" s="72">
         <v>6</v>
       </c>
-      <c r="K23" s="74" t="s">
+      <c r="K23" s="73" t="s">
         <v>18</v>
       </c>
       <c r="M23" s="33"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
+      <c r="A24" s="125"/>
       <c r="B24" s="30" t="s">
         <v>25</v>
       </c>
@@ -2131,10 +2133,10 @@
       <c r="E24" s="32">
         <v>0</v>
       </c>
-      <c r="F24" s="116" t="s">
+      <c r="F24" s="132" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="115"/>
+      <c r="G24" s="111"/>
       <c r="I24" s="43"/>
       <c r="J24" s="34">
         <v>7</v>
@@ -2143,7 +2145,7 @@
       <c r="M24" s="33"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="133"/>
+      <c r="A25" s="125"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25" t="s">
         <v>36</v>
@@ -2154,7 +2156,7 @@
       <c r="E25" s="26">
         <v>0</v>
       </c>
-      <c r="F25" s="117"/>
+      <c r="F25" s="133"/>
       <c r="I25" s="45"/>
       <c r="J25" s="41">
         <v>8</v>
@@ -2163,7 +2165,7 @@
       <c r="M25" s="33"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133"/>
+      <c r="A26" s="125"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28" t="s">
         <v>37</v>
@@ -2174,11 +2176,11 @@
       <c r="E26" s="29">
         <v>1</v>
       </c>
-      <c r="F26" s="118"/>
+      <c r="F26" s="134"/>
       <c r="M26" s="33"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="133"/>
+      <c r="A27" s="125"/>
       <c r="B27" s="30" t="s">
         <v>26</v>
       </c>
@@ -2191,12 +2193,12 @@
       <c r="E27" s="32">
         <v>0</v>
       </c>
-      <c r="F27" s="116" t="s">
+      <c r="F27" s="132" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="133"/>
+      <c r="A28" s="125"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25" t="s">
         <v>36</v>
@@ -2207,12 +2209,12 @@
       <c r="E28" s="26">
         <v>1</v>
       </c>
-      <c r="F28" s="117"/>
+      <c r="F28" s="133"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="133"/>
+      <c r="A29" s="125"/>
       <c r="B29" s="27"/>
       <c r="C29" s="28" t="s">
         <v>37</v>
@@ -2223,12 +2225,12 @@
       <c r="E29" s="29">
         <v>0</v>
       </c>
-      <c r="F29" s="118"/>
+      <c r="F29" s="134"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="133"/>
+      <c r="A30" s="125"/>
       <c r="B30" s="30" t="s">
         <v>27</v>
       </c>
@@ -2241,14 +2243,14 @@
       <c r="E30" s="32">
         <v>0</v>
       </c>
-      <c r="F30" s="116" t="s">
+      <c r="F30" s="132" t="s">
         <v>100</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="133"/>
+      <c r="A31" s="125"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25" t="s">
         <v>36</v>
@@ -2259,12 +2261,12 @@
       <c r="E31" s="26">
         <v>1</v>
       </c>
-      <c r="F31" s="117"/>
+      <c r="F31" s="133"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="133"/>
+      <c r="A32" s="125"/>
       <c r="B32" s="27"/>
       <c r="C32" s="28" t="s">
         <v>37</v>
@@ -2275,11 +2277,11 @@
       <c r="E32" s="29">
         <v>1</v>
       </c>
-      <c r="F32" s="118"/>
+      <c r="F32" s="134"/>
       <c r="M32" s="33"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="133"/>
+      <c r="A33" s="125"/>
       <c r="B33" s="30" t="s">
         <v>34</v>
       </c>
@@ -2292,7 +2294,7 @@
       <c r="E33" s="32">
         <v>1</v>
       </c>
-      <c r="F33" s="116" t="s">
+      <c r="F33" s="132" t="s">
         <v>97</v>
       </c>
       <c r="M33" s="33"/>
@@ -2300,7 +2302,7 @@
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="133"/>
+      <c r="A34" s="125"/>
       <c r="B34" s="24"/>
       <c r="C34" s="25" t="s">
         <v>36</v>
@@ -2311,11 +2313,11 @@
       <c r="E34" s="26">
         <v>0</v>
       </c>
-      <c r="F34" s="117"/>
+      <c r="F34" s="133"/>
       <c r="M34" s="33"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="133"/>
+      <c r="A35" s="125"/>
       <c r="B35" s="24"/>
       <c r="C35" s="25" t="s">
         <v>37</v>
@@ -2326,31 +2328,31 @@
       <c r="E35" s="26">
         <v>0</v>
       </c>
-      <c r="F35" s="118"/>
+      <c r="F35" s="134"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="97" t="s">
+      <c r="A36" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="99" t="s">
+      <c r="C36" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="99" t="s">
+      <c r="D36" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="100" t="s">
+      <c r="E36" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="106"/>
+      <c r="F36" s="102"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="127" t="s">
+      <c r="A37" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="63" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="60" t="s">
@@ -2359,44 +2361,44 @@
       <c r="D37" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="67">
-        <v>0</v>
-      </c>
-      <c r="F37" s="116" t="s">
+      <c r="E37" s="66">
+        <v>0</v>
+      </c>
+      <c r="F37" s="132" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="128"/>
-      <c r="B38" s="65"/>
+      <c r="A38" s="120"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="68">
-        <v>0</v>
-      </c>
-      <c r="F38" s="117"/>
+      <c r="E38" s="67">
+        <v>0</v>
+      </c>
+      <c r="F38" s="133"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="128"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="63" t="s">
+      <c r="A39" s="120"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E39" s="69">
-        <v>0</v>
-      </c>
-      <c r="F39" s="118"/>
+      <c r="E39" s="68">
+        <v>0</v>
+      </c>
+      <c r="F39" s="134"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="128"/>
-      <c r="B40" s="64" t="s">
+      <c r="A40" s="120"/>
+      <c r="B40" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="60" t="s">
@@ -2405,44 +2407,44 @@
       <c r="D40" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="67">
-        <v>0</v>
-      </c>
-      <c r="F40" s="116" t="s">
+      <c r="E40" s="66">
+        <v>0</v>
+      </c>
+      <c r="F40" s="132" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="128"/>
-      <c r="B41" s="65"/>
+      <c r="A41" s="120"/>
+      <c r="B41" s="64"/>
       <c r="C41" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="68">
-        <v>0</v>
-      </c>
-      <c r="F41" s="117"/>
+      <c r="E41" s="67">
+        <v>0</v>
+      </c>
+      <c r="F41" s="133"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="128"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="63" t="s">
+      <c r="A42" s="120"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="63" t="s">
+      <c r="D42" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="69">
+      <c r="E42" s="68">
         <v>1</v>
       </c>
-      <c r="F42" s="118"/>
+      <c r="F42" s="134"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="128"/>
-      <c r="B43" s="64" t="s">
+      <c r="A43" s="120"/>
+      <c r="B43" s="63" t="s">
         <v>29</v>
       </c>
       <c r="C43" s="60" t="s">
@@ -2451,44 +2453,44 @@
       <c r="D43" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="67">
-        <v>0</v>
-      </c>
-      <c r="F43" s="116" t="s">
+      <c r="E43" s="66">
+        <v>0</v>
+      </c>
+      <c r="F43" s="132" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="128"/>
-      <c r="B44" s="65"/>
+      <c r="A44" s="120"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="68">
+      <c r="E44" s="67">
         <v>1</v>
       </c>
-      <c r="F44" s="117"/>
+      <c r="F44" s="133"/>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="128"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="63" t="s">
+      <c r="A45" s="120"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="63" t="s">
+      <c r="D45" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="69">
-        <v>0</v>
-      </c>
-      <c r="F45" s="118"/>
+      <c r="E45" s="68">
+        <v>0</v>
+      </c>
+      <c r="F45" s="134"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="128"/>
-      <c r="B46" s="64" t="s">
+      <c r="A46" s="120"/>
+      <c r="B46" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="60" t="s">
@@ -2497,44 +2499,44 @@
       <c r="D46" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="67">
-        <v>0</v>
-      </c>
-      <c r="F46" s="116" t="s">
+      <c r="E46" s="66">
+        <v>0</v>
+      </c>
+      <c r="F46" s="132" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="128"/>
-      <c r="B47" s="65"/>
+      <c r="A47" s="120"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D47" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="68">
+      <c r="E47" s="67">
         <v>1</v>
       </c>
-      <c r="F47" s="117"/>
+      <c r="F47" s="133"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="128"/>
-      <c r="B48" s="66"/>
-      <c r="C48" s="63" t="s">
+      <c r="A48" s="120"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="63" t="s">
+      <c r="D48" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="69">
+      <c r="E48" s="68">
         <v>1</v>
       </c>
-      <c r="F48" s="118"/>
+      <c r="F48" s="134"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="128"/>
-      <c r="B49" s="64" t="s">
+      <c r="A49" s="120"/>
+      <c r="B49" s="63" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="60" t="s">
@@ -2543,43 +2545,43 @@
       <c r="D49" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="67">
+      <c r="E49" s="66">
         <v>1</v>
       </c>
-      <c r="F49" s="116" t="s">
+      <c r="F49" s="132" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="128"/>
-      <c r="B50" s="65"/>
+      <c r="A50" s="120"/>
+      <c r="B50" s="64"/>
       <c r="C50" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D50" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="68">
-        <v>0</v>
-      </c>
-      <c r="F50" s="117"/>
+      <c r="E50" s="67">
+        <v>0</v>
+      </c>
+      <c r="F50" s="133"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="128"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="63" t="s">
+      <c r="A51" s="120"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="63" t="s">
+      <c r="D51" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="E51" s="69">
-        <v>0</v>
-      </c>
-      <c r="F51" s="118"/>
+      <c r="E51" s="68">
+        <v>0</v>
+      </c>
+      <c r="F51" s="134"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="128"/>
+      <c r="A52" s="120"/>
       <c r="B52" s="61" t="s">
         <v>41</v>
       </c>
@@ -2589,15 +2591,15 @@
       <c r="D52" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="68">
+      <c r="E52" s="67">
         <v>1</v>
       </c>
-      <c r="F52" s="116" t="s">
+      <c r="F52" s="132" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="128"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="61"/>
       <c r="C53" s="59" t="s">
         <v>56</v>
@@ -2605,280 +2607,327 @@
       <c r="D53" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="68">
-        <v>0</v>
-      </c>
-      <c r="F53" s="117"/>
+      <c r="E53" s="67">
+        <v>0</v>
+      </c>
+      <c r="F53" s="133"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="129"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="63" t="s">
+      <c r="A54" s="121"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="63" t="s">
+      <c r="D54" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="E54" s="69">
+      <c r="E54" s="67">
         <v>1</v>
       </c>
-      <c r="F54" s="118"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="130" t="s">
+      <c r="F54" s="133"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="137"/>
+      <c r="B55" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="66">
+        <v>1</v>
+      </c>
+      <c r="F55" s="132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="137"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="67">
+        <v>1</v>
+      </c>
+      <c r="F56" s="133"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="137"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="68">
+        <v>0</v>
+      </c>
+      <c r="F57" s="134"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="102" t="s">
+      <c r="B58" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="103" t="s">
+      <c r="C58" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="103" t="s">
+      <c r="D58" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="E55" s="104">
-        <v>0</v>
-      </c>
-      <c r="F55" s="105" t="s">
+      <c r="E58" s="76">
+        <v>0</v>
+      </c>
+      <c r="F58" s="112" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="131"/>
-      <c r="B56" s="75" t="s">
+    <row r="59" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="123"/>
+      <c r="B59" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="76" t="s">
+      <c r="C59" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="76" t="s">
+      <c r="D59" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="77">
+      <c r="E59" s="76">
         <v>1</v>
       </c>
-      <c r="F56" s="107" t="s">
+      <c r="F59" s="103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="137" t="s">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="129" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="112" t="s">
+      <c r="B60" s="108" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="113" t="s">
+      <c r="C60" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D57" s="113" t="s">
+      <c r="D60" s="109" t="s">
         <v>128</v>
       </c>
-      <c r="E57" s="114">
-        <v>0</v>
-      </c>
-      <c r="F57" s="109" t="s">
+      <c r="E60" s="110">
+        <v>0</v>
+      </c>
+      <c r="F60" s="105" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="138"/>
-      <c r="B58" s="112" t="s">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="130"/>
+      <c r="B61" s="108" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="113" t="s">
+      <c r="C61" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="113" t="s">
+      <c r="D61" s="109" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="114">
+      <c r="E61" s="110">
         <v>1</v>
       </c>
-      <c r="F58" s="110" t="s">
+      <c r="F61" s="106" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="138"/>
-      <c r="B59" s="112" t="s">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="130"/>
+      <c r="B62" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="113" t="s">
+      <c r="C62" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="113" t="s">
+      <c r="D62" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="E59" s="114" t="s">
+      <c r="E62" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="F59" s="110"/>
-    </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="138"/>
-      <c r="B60" s="112" t="s">
+      <c r="F62" s="106"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="130"/>
+      <c r="B63" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="113" t="s">
+      <c r="C63" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="113" t="s">
+      <c r="D63" s="109" t="s">
         <v>126</v>
       </c>
-      <c r="E60" s="114" t="s">
+      <c r="E63" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="F60" s="110"/>
-    </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="138"/>
-      <c r="B61" s="112" t="s">
+      <c r="F63" s="106"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="130"/>
+      <c r="B64" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="113" t="s">
+      <c r="C64" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="113" t="s">
+      <c r="D64" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="E61" s="114" t="s">
+      <c r="E64" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="F61" s="110"/>
-    </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="139"/>
-      <c r="B62" s="112" t="s">
+      <c r="F64" s="106"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="131"/>
+      <c r="B65" s="108" t="s">
         <v>119</v>
       </c>
-      <c r="C62" s="113" t="s">
+      <c r="C65" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="113" t="s">
+      <c r="D65" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="E62" s="114" t="s">
+      <c r="E65" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="F62" s="111"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="124" t="s">
+      <c r="F65" s="107"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="81" t="s">
+      <c r="B66" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="82" t="s">
+      <c r="C66" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D66" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="83" t="s">
+      <c r="E66" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="F63" s="105"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="125"/>
-      <c r="B64" s="81" t="s">
+      <c r="F66" s="101"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="117"/>
+      <c r="B67" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C64" s="82" t="s">
+      <c r="C67" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="82" t="s">
+      <c r="D67" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="E64" s="83" t="s">
+      <c r="E67" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="F64" s="107"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="125"/>
-      <c r="B65" s="84" t="s">
+      <c r="F67" s="103"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="117"/>
+      <c r="B68" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="85" t="s">
+      <c r="C68" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="85" t="s">
+      <c r="D68" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="E65" s="94" t="s">
+      <c r="E68" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="F65" s="107"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="125"/>
-      <c r="B66" s="81" t="s">
+      <c r="F68" s="103"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="117"/>
+      <c r="B69" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="82" t="s">
+      <c r="C69" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="82" t="s">
+      <c r="D69" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="E66" s="87"/>
-      <c r="F66" s="106"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="125"/>
-      <c r="B67" s="84" t="s">
+      <c r="E69" s="86"/>
+      <c r="F69" s="102"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="117"/>
+      <c r="B70" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="85" t="s">
+      <c r="C70" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="85" t="s">
+      <c r="D70" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="86"/>
-      <c r="F67" s="108"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="125"/>
-      <c r="B68" s="81" t="s">
+      <c r="E70" s="85"/>
+      <c r="F70" s="104"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="117"/>
+      <c r="B71" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="82" t="s">
+      <c r="C71" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="82" t="s">
+      <c r="D71" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="E68" s="87"/>
-      <c r="F68" s="107"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="126"/>
-      <c r="B69" s="84" t="s">
+      <c r="E71" s="86"/>
+      <c r="F71" s="103"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="118"/>
+      <c r="B72" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="85" t="s">
+      <c r="C72" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="85" t="s">
+      <c r="D72" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="E69" s="86"/>
-      <c r="F69" s="108"/>
+      <c r="E72" s="85"/>
+      <c r="F72" s="104"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A63:A69"/>
-    <mergeCell ref="A37:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A21:A35"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A57:A62"/>
+  <mergeCells count="27">
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F49:F51"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
@@ -2891,13 +2940,13 @@
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A37:A54"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A21:A35"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A60:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Reformat of code ready for submission
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DesCon\DMM-STM32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amriksadhra/Development/Code/DMM-STM32/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="20440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
     <t>J7</t>
   </si>
@@ -420,13 +423,55 @@
   </si>
   <si>
     <t>(3&lt;&lt;5),~(1&lt;&lt;5)</t>
+  </si>
+  <si>
+    <t>Edge Connector Assignments</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>Mode switching pins on edge connector</t>
+  </si>
+  <si>
+    <t>Circuit selection pins on edge connector</t>
+  </si>
+  <si>
+    <t>ADC input pin on edge connector</t>
+  </si>
+  <si>
+    <t>Probe selection pins on edge connector</t>
+  </si>
+  <si>
+    <t>Capacitance autoranging pins</t>
+  </si>
+  <si>
+    <t>Diode test mode selection for diode test circuit</t>
+  </si>
+  <si>
+    <t>Diode test pins output from hardware into software</t>
+  </si>
+  <si>
+    <t>Signal generation pin in AF mode for DAC output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulse to trigger capacitance measuring </t>
+  </si>
+  <si>
+    <t>Pulse to measure capacitance pulse width from</t>
+  </si>
+  <si>
+    <t>HC-06 comms lines</t>
+  </si>
+  <si>
+    <t>FTDI232 comms lines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,6 +496,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -530,7 +591,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -540,26 +601,26 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -568,7 +629,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -576,22 +637,22 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,25 +661,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -626,23 +687,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -650,20 +711,20 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -673,206 +734,206 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,18 +941,33 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,9 +992,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1091,15 +1164,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1148,9 +1212,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1160,9 +1221,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1172,105 +1329,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFB9FF"/>
       <color rgb="FFF000F0"/>
-      <color rgb="FFFFB9FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1549,88 +1681,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="77" t="s">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="114" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="115" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="110">
+        <v>0</v>
+      </c>
+      <c r="F2" s="137" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="151" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J2" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K2" s="50" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="135" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="36">
-        <v>1</v>
-      </c>
-      <c r="K2" s="37"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114"/>
+    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="116"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>31</v>
@@ -1641,15 +1772,18 @@
       <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="34">
-        <v>2</v>
-      </c>
-      <c r="K3" s="39"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="114"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="148"/>
+      <c r="I3" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="35">
+        <v>1</v>
+      </c>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="116"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1662,19 +1796,18 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="135" t="s">
+      <c r="F4" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="55">
-        <v>3</v>
-      </c>
-      <c r="K4" s="58" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114"/>
+      <c r="G4" s="148"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="33">
+        <v>2</v>
+      </c>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="116"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>31</v>
@@ -1685,17 +1818,18 @@
       <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="55">
-        <v>4</v>
-      </c>
-      <c r="K5" s="58" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="148"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="54">
+        <v>3</v>
+      </c>
+      <c r="K5" s="57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="116"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1708,19 +1842,20 @@
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="135" t="s">
+      <c r="F6" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="55">
-        <v>5</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="114"/>
+      <c r="G6" s="148"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="54">
+        <v>4</v>
+      </c>
+      <c r="K6" s="57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="116"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
         <v>31</v>
@@ -1731,17 +1866,18 @@
       <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="136"/>
-      <c r="I7" s="38"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="148"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="54">
-        <v>6</v>
-      </c>
-      <c r="K7" s="71" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
+        <v>5</v>
+      </c>
+      <c r="K7" s="57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="116"/>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1754,19 +1890,20 @@
       <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="135" t="s">
+      <c r="F8" s="139" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="91">
-        <v>7</v>
-      </c>
-      <c r="K8" s="92" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="114"/>
+      <c r="G8" s="148"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="53">
+        <v>6</v>
+      </c>
+      <c r="K8" s="70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="116"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
         <v>31</v>
@@ -1777,15 +1914,18 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="136"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41">
-        <v>8</v>
-      </c>
-      <c r="K9" s="42"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="114"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="145"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="87">
+        <v>7</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="116"/>
       <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
@@ -1798,1128 +1938,1231 @@
       <c r="E10" s="11">
         <v>0</v>
       </c>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="36">
-        <v>1</v>
-      </c>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="115"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40">
+        <v>8</v>
+      </c>
+      <c r="K10" s="41"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="117"/>
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>1</v>
       </c>
-      <c r="F11" s="101" t="s">
+      <c r="F11" s="96" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="34">
+      <c r="G11" s="145"/>
+      <c r="I11" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="35">
+        <v>1</v>
+      </c>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="84"/>
+      <c r="C12" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="96"/>
+      <c r="G12" s="152" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="42"/>
+      <c r="J12" s="33">
         <v>2</v>
       </c>
-      <c r="K11" s="44"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="101"/>
-      <c r="G12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="94">
+      <c r="K12" s="43"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="134" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="157" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="J13" s="90">
         <v>3</v>
       </c>
-      <c r="K12" s="95" t="s">
+      <c r="K13" s="91" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="15" t="s">
+    <row r="14" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="129"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="136"/>
+      <c r="G14" s="148"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="68">
+        <v>4</v>
+      </c>
+      <c r="K14" s="69" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="129"/>
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="134" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="148"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="68">
+        <v>5</v>
+      </c>
+      <c r="K15" s="69" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="129"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1</v>
+      </c>
+      <c r="F16" s="136"/>
+      <c r="G16" s="148"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="68">
+        <v>6</v>
+      </c>
+      <c r="K16" s="69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="129"/>
+      <c r="B17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
+      <c r="F17" s="134" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="148"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="33">
+        <v>7</v>
+      </c>
+      <c r="K17" s="43"/>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="129"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="136"/>
+      <c r="G18" s="148"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="40">
+        <v>8</v>
+      </c>
+      <c r="K18" s="45"/>
+      <c r="M18" s="32"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="129"/>
+      <c r="B19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+      <c r="F19" s="134" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="148"/>
+      <c r="I19" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="35">
+        <v>1</v>
+      </c>
+      <c r="K19" s="47"/>
+      <c r="M19" s="32"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="130"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="19">
+        <v>1</v>
+      </c>
+      <c r="F20" s="136"/>
+      <c r="G20" s="145"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="51">
+        <v>2</v>
+      </c>
+      <c r="K20" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="32"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="126" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="25">
+        <v>0</v>
+      </c>
+      <c r="F21" s="134" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="155" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="42"/>
+      <c r="J21" s="51">
+        <v>3</v>
+      </c>
+      <c r="K21" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="32"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="127"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="135"/>
+      <c r="G22" s="148"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="55">
+        <v>4</v>
+      </c>
+      <c r="K22" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" s="32"/>
+    </row>
+    <row r="23" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="127"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="28">
+        <v>0</v>
+      </c>
+      <c r="F23" s="136"/>
+      <c r="G23" s="148"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="55">
+        <v>5</v>
+      </c>
+      <c r="K23" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="32"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="127"/>
+      <c r="B24" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="17">
-        <v>0</v>
-      </c>
-      <c r="F13" s="132" t="s">
-        <v>93</v>
-      </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="69">
-        <v>4</v>
-      </c>
-      <c r="K13" s="70" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="127"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="20">
-        <v>0</v>
-      </c>
-      <c r="F14" s="134"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="69">
-        <v>5</v>
-      </c>
-      <c r="K14" s="70" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="127"/>
-      <c r="B15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="17">
-        <v>0</v>
-      </c>
-      <c r="F15" s="132" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="69">
+      <c r="C24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="31">
+        <v>0</v>
+      </c>
+      <c r="F24" s="134" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="156"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="71">
         <v>6</v>
       </c>
-      <c r="K15" s="70" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="127"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="20">
+      <c r="K24" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="32"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="127"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="135"/>
+      <c r="G25" s="148"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="33">
+        <v>7</v>
+      </c>
+      <c r="K25" s="43"/>
+      <c r="M25" s="32"/>
+    </row>
+    <row r="26" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="127"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="134"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="34">
-        <v>7</v>
-      </c>
-      <c r="K16" s="44"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="17">
+      <c r="F26" s="136"/>
+      <c r="G26" s="148"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="40">
+        <v>8</v>
+      </c>
+      <c r="K26" s="45"/>
+      <c r="M26" s="32"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="127"/>
+      <c r="B27" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="31">
+        <v>0</v>
+      </c>
+      <c r="F27" s="134" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="148"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="127"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="25">
         <v>1</v>
       </c>
-      <c r="F17" s="132" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="41">
-        <v>8</v>
-      </c>
-      <c r="K17" s="46"/>
-      <c r="M17" s="33"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="127"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="20">
-        <v>0</v>
-      </c>
-      <c r="F18" s="134"/>
-      <c r="I18" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="36">
-        <v>1</v>
-      </c>
-      <c r="K18" s="48"/>
-      <c r="M18" s="33"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="127"/>
-      <c r="B19" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="23">
-        <v>1</v>
-      </c>
-      <c r="F19" s="132" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="52">
-        <v>2</v>
-      </c>
-      <c r="K19" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" s="33"/>
-    </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="128"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="134"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="52">
-        <v>3</v>
-      </c>
-      <c r="K20" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="33"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="124" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="26">
-        <v>0</v>
-      </c>
-      <c r="F21" s="132" t="s">
-        <v>98</v>
-      </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="56">
-        <v>4</v>
-      </c>
-      <c r="K21" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21" s="33"/>
-    </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="26">
-        <v>0</v>
-      </c>
-      <c r="F22" s="133"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="56">
-        <v>5</v>
-      </c>
-      <c r="K22" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="33"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="125"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="29">
-        <v>0</v>
-      </c>
-      <c r="F23" s="134"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="72">
-        <v>6</v>
-      </c>
-      <c r="K23" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="125"/>
-      <c r="B24" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="32">
-        <v>0</v>
-      </c>
-      <c r="F24" s="132" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="111"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="34">
-        <v>7</v>
-      </c>
-      <c r="K24" s="44"/>
-      <c r="M24" s="33"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="125"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="26">
-        <v>0</v>
-      </c>
-      <c r="F25" s="133"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="41">
-        <v>8</v>
-      </c>
-      <c r="K25" s="46"/>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="125"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="29">
-        <v>1</v>
-      </c>
-      <c r="F26" s="134"/>
-      <c r="M26" s="33"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="125"/>
-      <c r="B27" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="32">
-        <v>0</v>
-      </c>
-      <c r="F27" s="132" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="26">
-        <v>1</v>
-      </c>
-      <c r="F28" s="133"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="148"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="125"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28" t="s">
+    <row r="29" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="127"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="29">
-        <v>0</v>
-      </c>
-      <c r="F29" s="134"/>
+      <c r="E29" s="28">
+        <v>0</v>
+      </c>
+      <c r="F29" s="136"/>
+      <c r="G29" s="148"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
-      <c r="B30" s="30" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="127"/>
+      <c r="B30" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="32">
-        <v>0</v>
-      </c>
-      <c r="F30" s="132" t="s">
+      <c r="E30" s="31">
+        <v>0</v>
+      </c>
+      <c r="F30" s="134" t="s">
         <v>100</v>
       </c>
+      <c r="G30" s="148"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="127"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="25">
         <v>1</v>
       </c>
-      <c r="F31" s="133"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="148"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="125"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28" t="s">
+    <row r="32" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="127"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="28">
         <v>1</v>
       </c>
-      <c r="F32" s="134"/>
-      <c r="M32" s="33"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="125"/>
-      <c r="B33" s="30" t="s">
+      <c r="F32" s="136"/>
+      <c r="G32" s="148"/>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="127"/>
+      <c r="B33" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <v>1</v>
       </c>
-      <c r="F33" s="132" t="s">
+      <c r="F33" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="M33" s="33"/>
+      <c r="G33" s="148"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="125"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25" t="s">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="127"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="26">
-        <v>0</v>
-      </c>
-      <c r="F34" s="133"/>
-      <c r="M34" s="33"/>
-    </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="125"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25" t="s">
+      <c r="E34" s="25">
+        <v>0</v>
+      </c>
+      <c r="F34" s="135"/>
+      <c r="G34" s="148"/>
+      <c r="M34" s="32"/>
+    </row>
+    <row r="35" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="127"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="26">
-        <v>0</v>
-      </c>
-      <c r="F35" s="134"/>
-    </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="96" t="s">
+      <c r="E35" s="25">
+        <v>0</v>
+      </c>
+      <c r="F35" s="136"/>
+      <c r="G35" s="145"/>
+    </row>
+    <row r="36" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="97" t="s">
+      <c r="B36" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="98" t="s">
+      <c r="C36" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="98" t="s">
+      <c r="D36" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="99" t="s">
+      <c r="E36" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="102"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="119" t="s">
+      <c r="F36" s="97"/>
+      <c r="G36" s="92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="60" t="s">
+      <c r="C37" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="60" t="s">
+      <c r="D37" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="66">
-        <v>0</v>
-      </c>
-      <c r="F37" s="132" t="s">
+      <c r="E37" s="65">
+        <v>0</v>
+      </c>
+      <c r="F37" s="134" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="59" t="s">
+      <c r="G37" s="150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="122"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="67">
-        <v>0</v>
-      </c>
-      <c r="F38" s="133"/>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="120"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="62" t="s">
+      <c r="E38" s="66">
+        <v>0</v>
+      </c>
+      <c r="F38" s="135"/>
+      <c r="G38" s="148"/>
+    </row>
+    <row r="39" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="122"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D39" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E39" s="68">
-        <v>0</v>
-      </c>
-      <c r="F39" s="134"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
-      <c r="B40" s="63" t="s">
+      <c r="E39" s="67">
+        <v>0</v>
+      </c>
+      <c r="F39" s="136"/>
+      <c r="G39" s="148"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="122"/>
+      <c r="B40" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="66">
-        <v>0</v>
-      </c>
-      <c r="F40" s="132" t="s">
+      <c r="E40" s="65">
+        <v>0</v>
+      </c>
+      <c r="F40" s="134" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="59" t="s">
+      <c r="G40" s="148"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="122"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="67">
-        <v>0</v>
-      </c>
-      <c r="F41" s="133"/>
-    </row>
-    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="62" t="s">
+      <c r="E41" s="66">
+        <v>0</v>
+      </c>
+      <c r="F41" s="135"/>
+      <c r="G41" s="148"/>
+    </row>
+    <row r="42" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="122"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="62" t="s">
+      <c r="D42" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="68">
+      <c r="E42" s="67">
         <v>1</v>
       </c>
-      <c r="F42" s="134"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
-      <c r="B43" s="63" t="s">
+      <c r="F42" s="136"/>
+      <c r="G42" s="148"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="122"/>
+      <c r="B43" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="60" t="s">
+      <c r="C43" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="60" t="s">
+      <c r="D43" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="66">
-        <v>0</v>
-      </c>
-      <c r="F43" s="132" t="s">
+      <c r="E43" s="65">
+        <v>0</v>
+      </c>
+      <c r="F43" s="134" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="59" t="s">
+      <c r="G43" s="148"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="122"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="67">
+      <c r="E44" s="66">
         <v>1</v>
       </c>
-      <c r="F44" s="133"/>
-    </row>
-    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="120"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="62" t="s">
+      <c r="F44" s="135"/>
+      <c r="G44" s="148"/>
+    </row>
+    <row r="45" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="122"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="62" t="s">
+      <c r="D45" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="68">
-        <v>0</v>
-      </c>
-      <c r="F45" s="134"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="120"/>
-      <c r="B46" s="63" t="s">
+      <c r="E45" s="67">
+        <v>0</v>
+      </c>
+      <c r="F45" s="136"/>
+      <c r="G45" s="148"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="122"/>
+      <c r="B46" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="60" t="s">
+      <c r="C46" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="60" t="s">
+      <c r="D46" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="66">
-        <v>0</v>
-      </c>
-      <c r="F46" s="132" t="s">
+      <c r="E46" s="65">
+        <v>0</v>
+      </c>
+      <c r="F46" s="134" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="120"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="59" t="s">
+      <c r="G46" s="148"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="122"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D47" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="67">
+      <c r="E47" s="66">
         <v>1</v>
       </c>
-      <c r="F47" s="133"/>
-    </row>
-    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="120"/>
-      <c r="B48" s="65"/>
-      <c r="C48" s="62" t="s">
+      <c r="F47" s="135"/>
+      <c r="G47" s="148"/>
+    </row>
+    <row r="48" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="122"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="62" t="s">
+      <c r="D48" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="68">
+      <c r="E48" s="67">
         <v>1</v>
       </c>
-      <c r="F48" s="134"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="120"/>
-      <c r="B49" s="63" t="s">
+      <c r="F48" s="136"/>
+      <c r="G48" s="148"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="122"/>
+      <c r="B49" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="60" t="s">
+      <c r="C49" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="60" t="s">
+      <c r="D49" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="66">
+      <c r="E49" s="65">
         <v>1</v>
       </c>
-      <c r="F49" s="132" t="s">
+      <c r="F49" s="134" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="120"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="59" t="s">
+      <c r="G49" s="148"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="122"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="59" t="s">
+      <c r="D50" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="67">
-        <v>0</v>
-      </c>
-      <c r="F50" s="133"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="120"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="62" t="s">
+      <c r="E50" s="66">
+        <v>0</v>
+      </c>
+      <c r="F50" s="135"/>
+      <c r="G50" s="148"/>
+    </row>
+    <row r="51" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="122"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="62" t="s">
+      <c r="D51" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E51" s="68">
-        <v>0</v>
-      </c>
-      <c r="F51" s="134"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="120"/>
-      <c r="B52" s="61" t="s">
+      <c r="E51" s="67">
+        <v>0</v>
+      </c>
+      <c r="F51" s="136"/>
+      <c r="G51" s="148"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="122"/>
+      <c r="B52" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="59" t="s">
+      <c r="D52" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="67">
+      <c r="E52" s="66">
         <v>1</v>
       </c>
-      <c r="F52" s="132" t="s">
+      <c r="F52" s="134" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="120"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="59" t="s">
+      <c r="G52" s="148"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="122"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="59" t="s">
+      <c r="D53" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="67">
-        <v>0</v>
-      </c>
-      <c r="F53" s="133"/>
-    </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="121"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="59" t="s">
+      <c r="E53" s="66">
+        <v>0</v>
+      </c>
+      <c r="F53" s="135"/>
+      <c r="G53" s="148"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="123"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="59" t="s">
+      <c r="D54" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="E54" s="67">
+      <c r="E54" s="66">
         <v>1</v>
       </c>
-      <c r="F54" s="133"/>
-    </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="137"/>
-      <c r="B55" s="63" t="s">
+      <c r="F54" s="135"/>
+      <c r="G54" s="148"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="106"/>
+      <c r="B55" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C55" s="60" t="s">
+      <c r="C55" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="60" t="s">
+      <c r="D55" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="E55" s="66">
+      <c r="E55" s="65">
         <v>1</v>
       </c>
-      <c r="F55" s="132" t="s">
+      <c r="F55" s="134" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="137"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="59" t="s">
+      <c r="G55" s="148"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="106"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="59" t="s">
+      <c r="D56" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="67">
+      <c r="E56" s="66">
         <v>1</v>
       </c>
-      <c r="F56" s="133"/>
-    </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="137"/>
-      <c r="B57" s="65"/>
-      <c r="C57" s="62" t="s">
+      <c r="F56" s="135"/>
+      <c r="G56" s="148"/>
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="106"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="62" t="s">
+      <c r="D57" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="68">
-        <v>0</v>
-      </c>
-      <c r="F57" s="134"/>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="122" t="s">
+      <c r="E57" s="67">
+        <v>0</v>
+      </c>
+      <c r="F57" s="136"/>
+      <c r="G57" s="145"/>
+    </row>
+    <row r="58" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="138" t="s">
+      <c r="B58" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="75" t="s">
+      <c r="C58" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="75" t="s">
+      <c r="D58" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="76">
-        <v>0</v>
-      </c>
-      <c r="F58" s="112" t="s">
+      <c r="E58" s="75">
+        <v>0</v>
+      </c>
+      <c r="F58" s="105" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="123"/>
-      <c r="B59" s="74" t="s">
+      <c r="G58" s="154" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="125"/>
+      <c r="B59" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="75" t="s">
+      <c r="C59" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="75" t="s">
+      <c r="D59" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="E59" s="76">
+      <c r="E59" s="75">
         <v>1</v>
       </c>
-      <c r="F59" s="103" t="s">
+      <c r="F59" s="98" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="129" t="s">
+      <c r="G59" s="145"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="131" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="108" t="s">
+      <c r="B60" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="109" t="s">
+      <c r="C60" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="109" t="s">
+      <c r="D60" s="103" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="110">
-        <v>0</v>
-      </c>
-      <c r="F60" s="105" t="s">
+      <c r="E60" s="104">
+        <v>0</v>
+      </c>
+      <c r="F60" s="99" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="130"/>
-      <c r="B61" s="108" t="s">
+      <c r="G60" s="147" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="132"/>
+      <c r="B61" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="109" t="s">
+      <c r="C61" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="109" t="s">
+      <c r="D61" s="103" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="110">
+      <c r="E61" s="104">
         <v>1</v>
       </c>
-      <c r="F61" s="106" t="s">
+      <c r="F61" s="100" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="130"/>
-      <c r="B62" s="108" t="s">
+      <c r="G61" s="148"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="132"/>
+      <c r="B62" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="109" t="s">
+      <c r="C62" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="109" t="s">
+      <c r="D62" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="110" t="s">
+      <c r="E62" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="F62" s="106"/>
-    </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="130"/>
-      <c r="B63" s="108" t="s">
+      <c r="F62" s="100"/>
+      <c r="G62" s="149" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="132"/>
+      <c r="B63" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="C63" s="109" t="s">
+      <c r="C63" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="109" t="s">
+      <c r="D63" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="E63" s="110" t="s">
+      <c r="E63" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="F63" s="106"/>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="130"/>
-      <c r="B64" s="108" t="s">
+      <c r="F63" s="100"/>
+      <c r="G63" s="148"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="132"/>
+      <c r="B64" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="109" t="s">
+      <c r="C64" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="109" t="s">
+      <c r="D64" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="E64" s="110" t="s">
+      <c r="E64" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="F64" s="106"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="131"/>
-      <c r="B65" s="108" t="s">
+      <c r="F64" s="100"/>
+      <c r="G64" s="148"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="133"/>
+      <c r="B65" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="C65" s="109" t="s">
+      <c r="C65" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="109" t="s">
+      <c r="D65" s="103" t="s">
         <v>124</v>
       </c>
-      <c r="E65" s="110" t="s">
+      <c r="E65" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="F65" s="107"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="116" t="s">
+      <c r="F65" s="101"/>
+      <c r="G65" s="145"/>
+    </row>
+    <row r="66" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="80" t="s">
+      <c r="B66" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="81" t="s">
+      <c r="D66" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="82" t="s">
+      <c r="E66" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="F66" s="101"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="117"/>
-      <c r="B67" s="80" t="s">
+      <c r="F66" s="142" t="s">
+        <v>133</v>
+      </c>
+      <c r="G66" s="143" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="119"/>
+      <c r="B67" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="81" t="s">
+      <c r="D67" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="E67" s="82" t="s">
+      <c r="E67" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="F67" s="103"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="117"/>
-      <c r="B68" s="83" t="s">
+      <c r="F67" s="140"/>
+      <c r="G67" s="144" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="119"/>
+      <c r="B68" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="84" t="s">
+      <c r="C68" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="84" t="s">
+      <c r="D68" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="E68" s="93" t="s">
+      <c r="E68" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="103"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="117"/>
-      <c r="B69" s="80" t="s">
+      <c r="F68" s="140"/>
+      <c r="G68" s="144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="119"/>
+      <c r="B69" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D69" s="81" t="s">
+      <c r="D69" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="86"/>
-      <c r="F69" s="102"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="117"/>
-      <c r="B70" s="83" t="s">
+      <c r="E69" s="82"/>
+      <c r="F69" s="146" t="s">
+        <v>133</v>
+      </c>
+      <c r="G69" s="144" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="119"/>
+      <c r="B70" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="C70" s="84" t="s">
+      <c r="C70" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D70" s="84" t="s">
+      <c r="D70" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="E70" s="85"/>
-      <c r="F70" s="104"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="117"/>
-      <c r="B71" s="80" t="s">
+      <c r="E70" s="81"/>
+      <c r="F70" s="141" t="s">
+        <v>133</v>
+      </c>
+      <c r="G70" s="148"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="119"/>
+      <c r="B71" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="81" t="s">
+      <c r="C71" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="D71" s="81" t="s">
+      <c r="D71" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="E71" s="86"/>
-      <c r="F71" s="103"/>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="118"/>
-      <c r="B72" s="83" t="s">
+      <c r="E71" s="82"/>
+      <c r="F71" s="140" t="s">
+        <v>133</v>
+      </c>
+      <c r="G71" s="153" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="120"/>
+      <c r="B72" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="84" t="s">
+      <c r="C72" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D72" s="84" t="s">
+      <c r="D72" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="85"/>
-      <c r="F72" s="104"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="141" t="s">
+        <v>133</v>
+      </c>
+      <c r="G72" s="145"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F27:F29"/>
     <mergeCell ref="F55:F57"/>
     <mergeCell ref="F52:F54"/>
     <mergeCell ref="F33:F35"/>
@@ -2928,6 +3171,14 @@
     <mergeCell ref="F43:F45"/>
     <mergeCell ref="F46:F48"/>
     <mergeCell ref="F49:F51"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A37:A54"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A21:A35"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A60:A65"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
@@ -2936,17 +3187,6 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A37:A54"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A21:A35"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A60:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>